<commit_message>
# SENSOR_DATA를 매 block 마다 삽입
</commit_message>
<xml_diff>
--- a/xlsx/5x5_data_blocks_with_gaps.xlsx
+++ b/xlsx/5x5_data_blocks_with_gaps.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,87 +423,87 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B1" t="n">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C1" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" t="n">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="E1" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="D2" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E2" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="C3" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E3" t="n">
-        <v>85</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B4" t="n">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="D4" t="n">
+        <v>86</v>
+      </c>
+      <c r="E4" t="n">
         <v>53</v>
-      </c>
-      <c r="E4" t="n">
-        <v>95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="B5" t="n">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C5" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D5" t="n">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="E5" t="n">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -515,153 +515,565 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>96</v>
+        <v>29</v>
       </c>
       <c r="B7" t="n">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="C7" t="n">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D7" t="n">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="E7" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="B8" t="n">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C8" t="n">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="D8" t="n">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="E9" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B10" t="n">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C10" t="n">
+        <v>39</v>
+      </c>
+      <c r="D10" t="n">
+        <v>99</v>
+      </c>
+      <c r="E10" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>30</v>
+      </c>
+      <c r="B11" t="n">
+        <v>78</v>
+      </c>
+      <c r="C11" t="n">
+        <v>12</v>
+      </c>
+      <c r="D11" t="n">
         <v>55</v>
       </c>
-      <c r="D10" t="n">
-        <v>84</v>
-      </c>
-      <c r="E10" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>80</v>
-      </c>
-      <c r="B12" t="n">
-        <v>55</v>
-      </c>
-      <c r="C12" t="n">
-        <v>26</v>
-      </c>
-      <c r="D12" t="n">
-        <v>49</v>
-      </c>
-      <c r="E12" t="n">
-        <v>76</v>
-      </c>
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B13" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>61</v>
       </c>
       <c r="D13" t="n">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="E13" t="n">
-        <v>3</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B14" t="n">
+        <v>79</v>
+      </c>
+      <c r="C14" t="n">
         <v>2</v>
       </c>
-      <c r="C14" t="n">
-        <v>99</v>
-      </c>
       <c r="D14" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E14" t="n">
-        <v>87</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
+        <v>61</v>
+      </c>
+      <c r="B15" t="n">
+        <v>38</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" t="n">
+        <v>97</v>
+      </c>
+      <c r="E15" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>6</v>
+      </c>
+      <c r="B16" t="n">
+        <v>21</v>
+      </c>
+      <c r="C16" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" t="n">
+        <v>58</v>
+      </c>
+      <c r="E16" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>76</v>
+      </c>
+      <c r="B17" t="n">
+        <v>69</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="n">
+        <v>79</v>
+      </c>
+      <c r="E17" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>94</v>
+      </c>
+      <c r="B19" t="n">
+        <v>10</v>
+      </c>
+      <c r="C19" t="n">
+        <v>46</v>
+      </c>
+      <c r="D19" t="n">
+        <v>70</v>
+      </c>
+      <c r="E19" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>85</v>
+      </c>
+      <c r="B20" t="n">
+        <v>51</v>
+      </c>
+      <c r="C20" t="n">
+        <v>45</v>
+      </c>
+      <c r="D20" t="n">
+        <v>91</v>
+      </c>
+      <c r="E20" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>69</v>
+      </c>
+      <c r="B21" t="n">
+        <v>54</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>99</v>
+      </c>
+      <c r="B22" t="n">
+        <v>54</v>
+      </c>
+      <c r="C22" t="n">
+        <v>33</v>
+      </c>
+      <c r="D22" t="n">
+        <v>48</v>
+      </c>
+      <c r="E22" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>35</v>
+      </c>
+      <c r="B23" t="n">
+        <v>62</v>
+      </c>
+      <c r="C23" t="n">
+        <v>36</v>
+      </c>
+      <c r="D23" t="n">
+        <v>84</v>
+      </c>
+      <c r="E23" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="n">
+        <v>62</v>
+      </c>
+      <c r="C25" t="n">
+        <v>63</v>
+      </c>
+      <c r="D25" t="n">
+        <v>37</v>
+      </c>
+      <c r="E25" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>4</v>
+      </c>
+      <c r="B26" t="n">
+        <v>56</v>
+      </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="n">
+        <v>93</v>
+      </c>
+      <c r="E26" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>60</v>
+      </c>
+      <c r="B27" t="n">
+        <v>89</v>
+      </c>
+      <c r="C27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" t="n">
+        <v>85</v>
+      </c>
+      <c r="E27" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>94</v>
+      </c>
+      <c r="B28" t="n">
+        <v>30</v>
+      </c>
+      <c r="C28" t="n">
+        <v>7</v>
+      </c>
+      <c r="D28" t="n">
+        <v>90</v>
+      </c>
+      <c r="E28" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>92</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>69</v>
+      </c>
+      <c r="D29" t="n">
+        <v>91</v>
+      </c>
+      <c r="E29" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>76</v>
+      </c>
+      <c r="B31" t="n">
+        <v>67</v>
+      </c>
+      <c r="C31" t="n">
+        <v>53</v>
+      </c>
+      <c r="D31" t="n">
+        <v>48</v>
+      </c>
+      <c r="E31" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>60</v>
+      </c>
+      <c r="B32" t="n">
+        <v>97</v>
+      </c>
+      <c r="C32" t="n">
+        <v>94</v>
+      </c>
+      <c r="D32" t="n">
+        <v>88</v>
+      </c>
+      <c r="E32" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>27</v>
+      </c>
+      <c r="B33" t="n">
         <v>82</v>
       </c>
-      <c r="B15" t="n">
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="n">
+        <v>68</v>
+      </c>
+      <c r="E33" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>51</v>
+      </c>
+      <c r="B34" t="n">
+        <v>85</v>
+      </c>
+      <c r="C34" t="n">
+        <v>33</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7</v>
+      </c>
+      <c r="E34" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>67</v>
+      </c>
+      <c r="B35" t="n">
+        <v>62</v>
+      </c>
+      <c r="C35" t="n">
+        <v>37</v>
+      </c>
+      <c r="D35" t="n">
+        <v>93</v>
+      </c>
+      <c r="E35" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>61</v>
+      </c>
+      <c r="B37" t="n">
+        <v>24</v>
+      </c>
+      <c r="C37" t="n">
+        <v>51</v>
+      </c>
+      <c r="D37" t="n">
+        <v>68</v>
+      </c>
+      <c r="E37" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>85</v>
+      </c>
+      <c r="B38" t="n">
+        <v>41</v>
+      </c>
+      <c r="C38" t="n">
+        <v>23</v>
+      </c>
+      <c r="D38" t="n">
+        <v>24</v>
+      </c>
+      <c r="E38" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>6</v>
+      </c>
+      <c r="B39" t="n">
+        <v>13</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>4</v>
+      </c>
+      <c r="E39" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>77</v>
+      </c>
+      <c r="B40" t="n">
+        <v>73</v>
+      </c>
+      <c r="C40" t="n">
+        <v>45</v>
+      </c>
+      <c r="D40" t="n">
+        <v>83</v>
+      </c>
+      <c r="E40" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>41</v>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+      <c r="C41" t="n">
         <v>86</v>
       </c>
-      <c r="C15" t="n">
-        <v>6</v>
-      </c>
-      <c r="D15" t="n">
-        <v>39</v>
-      </c>
-      <c r="E15" t="n">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>11</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>22</v>
+      </c>
+      <c r="B42" t="n">
+        <v>21</v>
+      </c>
+      <c r="C42" t="n">
+        <v>76</v>
+      </c>
+      <c r="D42" t="n">
+        <v>62</v>
+      </c>
+      <c r="E42" t="n">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
write a excel file and read it then plot (2,2) sensor data seems ok
</commit_message>
<xml_diff>
--- a/xlsx/5x5_data_blocks_with_gaps.xlsx
+++ b/xlsx/5x5_data_blocks_with_gaps.xlsx
@@ -423,87 +423,87 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>20</v>
+        <v>-2</v>
       </c>
       <c r="B1" t="n">
-        <v>27</v>
+        <v>-2</v>
       </c>
       <c r="C1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D1" t="n">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="E1" t="n">
-        <v>49</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>85</v>
+        <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>61</v>
+        <v>-2</v>
       </c>
       <c r="D2" t="n">
-        <v>48</v>
+        <v>-2</v>
       </c>
       <c r="E2" t="n">
-        <v>40</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>54</v>
+        <v>-1</v>
       </c>
       <c r="B3" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>95</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="D4" t="n">
-        <v>86</v>
+        <v>-1</v>
       </c>
       <c r="E4" t="n">
-        <v>53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>37</v>
+        <v>-2</v>
       </c>
       <c r="D5" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>22</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6">
@@ -515,87 +515,87 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
       <c r="B7" t="n">
-        <v>86</v>
+        <v>-2</v>
       </c>
       <c r="C7" t="n">
-        <v>64</v>
+        <v>-2</v>
       </c>
       <c r="D7" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>43</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B8" t="n">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="E8" t="n">
-        <v>74</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>19</v>
+        <v>-1</v>
       </c>
       <c r="B9" t="n">
-        <v>100</v>
+        <v>-1</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>15</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>19</v>
+        <v>-2</v>
       </c>
       <c r="B10" t="n">
-        <v>63</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>39</v>
+        <v>-2</v>
       </c>
       <c r="D10" t="n">
-        <v>99</v>
+        <v>-1</v>
       </c>
       <c r="E10" t="n">
-        <v>54</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B11" t="n">
-        <v>78</v>
+        <v>-2</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>46</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12">
@@ -607,87 +607,87 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B13" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>61</v>
+        <v>-2</v>
       </c>
       <c r="D13" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>96</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="B14" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="B15" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C15" t="n">
         <v>3</v>
       </c>
       <c r="D15" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B16" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>58</v>
+        <v>-1</v>
       </c>
       <c r="E16" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>76</v>
+        <v>-2</v>
       </c>
       <c r="B17" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>79</v>
+        <v>-2</v>
       </c>
       <c r="E17" t="n">
-        <v>83</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -699,87 +699,87 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>94</v>
+        <v>-2</v>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>46</v>
+        <v>-2</v>
       </c>
       <c r="D19" t="n">
-        <v>70</v>
+        <v>-1</v>
       </c>
       <c r="E19" t="n">
-        <v>81</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>85</v>
+        <v>-2</v>
       </c>
       <c r="B20" t="n">
-        <v>51</v>
+        <v>-2</v>
       </c>
       <c r="C20" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>91</v>
+        <v>-2</v>
       </c>
       <c r="E20" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>69</v>
+        <v>-1</v>
       </c>
       <c r="B21" t="n">
-        <v>54</v>
+        <v>-1</v>
       </c>
       <c r="C21" t="n">
         <v>2</v>
       </c>
       <c r="D21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="B22" t="n">
-        <v>54</v>
+        <v>-2</v>
       </c>
       <c r="C22" t="n">
-        <v>33</v>
+        <v>-1</v>
       </c>
       <c r="D22" t="n">
-        <v>48</v>
+        <v>-1</v>
       </c>
       <c r="E22" t="n">
-        <v>6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B23" t="n">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>36</v>
+        <v>-2</v>
       </c>
       <c r="D23" t="n">
-        <v>84</v>
+        <v>-2</v>
       </c>
       <c r="E23" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24">
@@ -791,87 +791,87 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>-1</v>
       </c>
       <c r="B25" t="n">
-        <v>62</v>
+        <v>-2</v>
       </c>
       <c r="C25" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B26" t="n">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="C26" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>93</v>
+        <v>-2</v>
       </c>
       <c r="E26" t="n">
-        <v>77</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>60</v>
+        <v>-2</v>
       </c>
       <c r="B27" t="n">
-        <v>89</v>
+        <v>-1</v>
       </c>
       <c r="C27" t="n">
         <v>3</v>
       </c>
       <c r="D27" t="n">
-        <v>85</v>
+        <v>-2</v>
       </c>
       <c r="E27" t="n">
-        <v>84</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="B28" t="n">
-        <v>30</v>
+        <v>-1</v>
       </c>
       <c r="C28" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>92</v>
+        <v>1</v>
       </c>
       <c r="B29" t="n">
-        <v>28</v>
+        <v>-1</v>
       </c>
       <c r="C29" t="n">
-        <v>69</v>
+        <v>-1</v>
       </c>
       <c r="D29" t="n">
-        <v>91</v>
+        <v>1</v>
       </c>
       <c r="E29" t="n">
-        <v>30</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30">
@@ -883,87 +883,87 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>76</v>
+        <v>-2</v>
       </c>
       <c r="B31" t="n">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D31" t="n">
-        <v>48</v>
+        <v>-1</v>
       </c>
       <c r="E31" t="n">
-        <v>23</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>60</v>
+        <v>-2</v>
       </c>
       <c r="B32" t="n">
-        <v>97</v>
+        <v>-1</v>
       </c>
       <c r="C32" t="n">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="D32" t="n">
-        <v>88</v>
+        <v>1</v>
       </c>
       <c r="E32" t="n">
-        <v>97</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B33" t="n">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="C33" t="n">
         <v>1</v>
       </c>
       <c r="D33" t="n">
-        <v>68</v>
+        <v>-2</v>
       </c>
       <c r="E33" t="n">
-        <v>9</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>51</v>
+        <v>-2</v>
       </c>
       <c r="B34" t="n">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>33</v>
+        <v>-2</v>
       </c>
       <c r="D34" t="n">
-        <v>7</v>
+        <v>-2</v>
       </c>
       <c r="E34" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="B35" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="C35" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>93</v>
+        <v>-2</v>
       </c>
       <c r="E35" t="n">
-        <v>47</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="36">
@@ -975,105 +975,95 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>61</v>
+        <v>-1</v>
       </c>
       <c r="B37" t="n">
-        <v>24</v>
+        <v>-1</v>
       </c>
       <c r="C37" t="n">
-        <v>51</v>
+        <v>1</v>
       </c>
       <c r="D37" t="n">
-        <v>68</v>
+        <v>-1</v>
       </c>
       <c r="E37" t="n">
-        <v>71</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="B38" t="n">
-        <v>41</v>
+        <v>-1</v>
       </c>
       <c r="C38" t="n">
-        <v>23</v>
+        <v>-1</v>
       </c>
       <c r="D38" t="n">
-        <v>24</v>
+        <v>-2</v>
       </c>
       <c r="E38" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B39" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>4</v>
+        <v>-2</v>
       </c>
       <c r="E39" t="n">
-        <v>28</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>77</v>
+        <v>-1</v>
       </c>
       <c r="B40" t="n">
-        <v>73</v>
+        <v>-1</v>
       </c>
       <c r="C40" t="n">
-        <v>45</v>
+        <v>-1</v>
       </c>
       <c r="D40" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>21</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>41</v>
+        <v>-1</v>
       </c>
       <c r="B41" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C41" t="n">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n">
-        <v>22</v>
-      </c>
-      <c r="B42" t="n">
-        <v>21</v>
-      </c>
-      <c r="C42" t="n">
-        <v>76</v>
-      </c>
-      <c r="D42" t="n">
-        <v>62</v>
-      </c>
-      <c r="E42" t="n">
-        <v>8</v>
-      </c>
+      <c r="A42" t="inlineStr"/>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>